<commit_message>
Commentato via "a" dal main per evitare confusione
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/output_ridotto.xlsx
+++ b/PS-VRP/Dati_output/output_ridotto.xlsx
@@ -38,14 +38,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CCE5FF"/>
-        <bgColor rgb="00CCE5FF"/>
+        <fgColor rgb="00F4CCCC"/>
+        <bgColor rgb="00F4CCCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00E2EFDA"/>
-        <bgColor rgb="00E2EFDA"/>
+        <fgColor rgb="00D9D2E9"/>
+        <bgColor rgb="00D9D2E9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00D5E8D4"/>
+        <bgColor rgb="00D5E8D4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FCE5CD"/>
+        <bgColor rgb="00FCE5CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CCE5FF"/>
+        <bgColor rgb="00CCE5FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -56,32 +74,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00D9D2E9"/>
-        <bgColor rgb="00D9D2E9"/>
+        <fgColor rgb="00FFF2CC"/>
+        <bgColor rgb="00FFF2CC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F4CCCC"/>
-        <bgColor rgb="00F4CCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FCE5CD"/>
-        <bgColor rgb="00FCE5CD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00D5E8D4"/>
-        <bgColor rgb="00D5E8D4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FFF2CC"/>
-        <bgColor rgb="00FFF2CC"/>
+        <fgColor rgb="00E2EFDA"/>
+        <bgColor rgb="00E2EFDA"/>
       </patternFill>
     </fill>
   </fills>

</xml_diff>

<commit_message>
Piccoli aggiustamenti pt. 3
</commit_message>
<xml_diff>
--- a/PS-VRP/Dati_output/output_ridotto.xlsx
+++ b/PS-VRP/Dati_output/output_ridotto.xlsx
@@ -38,6 +38,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="00D5E8D4"/>
+        <bgColor rgb="00D5E8D4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F4CCCC"/>
+        <bgColor rgb="00F4CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF2CC"/>
+        <bgColor rgb="00FFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00E2EFDA"/>
         <bgColor rgb="00E2EFDA"/>
       </patternFill>
@@ -50,14 +68,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F4CCCC"/>
-        <bgColor rgb="00F4CCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00CCE5FF"/>
-        <bgColor rgb="00CCE5FF"/>
+        <fgColor rgb="00FCE5CD"/>
+        <bgColor rgb="00FCE5CD"/>
       </patternFill>
     </fill>
     <fill>
@@ -68,20 +80,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFF2CC"/>
-        <bgColor rgb="00FFF2CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00D5E8D4"/>
-        <bgColor rgb="00D5E8D4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00FCE5CD"/>
-        <bgColor rgb="00FCE5CD"/>
+        <fgColor rgb="00CCE5FF"/>
+        <bgColor rgb="00CCE5FF"/>
       </patternFill>
     </fill>
   </fills>

</xml_diff>